<commit_message>
quick update on f patterns, rec devs, and starting on feeding data into wham inputs
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CC53C0-9E44-AA46-8592-03339251AFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97AA892-B768-F84F-ABFC-D9E2AE9969FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30060" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Number of years</t>
-  </si>
-  <si>
     <t>Number of simulations</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Recruitment at unfished equilibrium (taken from starting values of .dat file) - exponentiated</t>
+  </si>
+  <si>
+    <t>Number of years (clipping off the last year)</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +583,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,21 +591,21 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1600</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +625,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -636,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -801,100 +801,100 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>2.2375362999999999E-2</v>
@@ -1013,100 +1013,100 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>46</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1.2128000000000001</v>
@@ -1235,46 +1235,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0.59950000000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>20.085540000000002</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>246.28489999999999</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>1.2</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates on wham testing. new fxns on preparing inputs, sampling from fishery and survey
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97AA892-B768-F84F-ABFC-D9E2AE9969FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4F4894-3586-C643-A29D-AF9945625E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Weight_At_Age" sheetId="5" r:id="rId4"/>
     <sheet name="Recruitment" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -202,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +212,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,8 +244,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -602,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1600</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -618,7 +626,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1214,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,6 +1285,9 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug fixes should be operational now! OM-EM combination returns resutls as expected
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4F4894-3586-C643-A29D-AF9945625E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C891393A-B6D1-F448-AB43-AC61E6A75D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
     <sheet name="Age_Bins" sheetId="2" r:id="rId2"/>
     <sheet name="Maturity_At_Age" sheetId="4" r:id="rId3"/>
     <sheet name="Weight_At_Age" sheetId="5" r:id="rId4"/>
-    <sheet name="Recruitment" sheetId="6" r:id="rId5"/>
+    <sheet name="Recruitment_Mortality" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Par</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>Number of years (clipping off the last year)</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Natural Mortality</t>
+  </si>
+  <si>
+    <t>Mean recruitment</t>
+  </si>
+  <si>
+    <t>mu_rec</t>
   </si>
 </sst>
 </file>
@@ -564,7 +576,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1222,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1279,14 +1291,33 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1.2</v>
+        <v>0.75</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>16.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
updating general age structued assessment
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C891393A-B6D1-F448-AB43-AC61E6A75D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC16709-11F8-CD4A-9362-1F56C97BAFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>Par</t>
   </si>
@@ -208,6 +208,21 @@
   </si>
   <si>
     <t>mu_rec</t>
+  </si>
+  <si>
+    <t>n_sex</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Number of sexes (1. = Females, 2 = Males)</t>
+  </si>
+  <si>
+    <t>n_fleets</t>
+  </si>
+  <si>
+    <t>Number of fishery fleets</t>
   </si>
 </sst>
 </file>
@@ -573,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -626,6 +641,28 @@
       </c>
       <c r="C4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -811,15 +848,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D3" sqref="D3:AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -827,97 +864,100 @@
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -925,93 +965,197 @@
         <v>49</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>2.2375362999999999E-2</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.6018622000000002E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>9.2286517999999998E-2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.176467916</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.31111834199999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.48767028899999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.66735326100000003</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.80873412499999997</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.89910986100000001</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.94945097899999997</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.97536173299999995</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.98815665200000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.99434555199999997</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.99730916599999997</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.99872148500000002</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.99939298099999996</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.99971189900000001</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.99986328499999999</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>0.99993512900000003</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>0.99996921999999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>0.99998539600000003</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>0.99999307100000001</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>0.99999671199999995</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>0.99999844000000004</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>0.99999925999999995</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>0.99999964900000005</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>0.99999983299999995</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>0.99999992100000001</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>0.99999996199999996</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
+        <v>0.99999998199999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2.2375362999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.6018622000000002E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.2286517999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.176467916</v>
+      </c>
+      <c r="H3">
+        <v>0.31111834199999999</v>
+      </c>
+      <c r="I3">
+        <v>0.48767028899999998</v>
+      </c>
+      <c r="J3">
+        <v>0.66735326100000003</v>
+      </c>
+      <c r="K3">
+        <v>0.80873412499999997</v>
+      </c>
+      <c r="L3">
+        <v>0.89910986100000001</v>
+      </c>
+      <c r="M3">
+        <v>0.94945097899999997</v>
+      </c>
+      <c r="N3">
+        <v>0.97536173299999995</v>
+      </c>
+      <c r="O3">
+        <v>0.98815665200000002</v>
+      </c>
+      <c r="P3">
+        <v>0.99434555199999997</v>
+      </c>
+      <c r="Q3">
+        <v>0.99730916599999997</v>
+      </c>
+      <c r="R3">
+        <v>0.99872148500000002</v>
+      </c>
+      <c r="S3">
+        <v>0.99939298099999996</v>
+      </c>
+      <c r="T3">
+        <v>0.99971189900000001</v>
+      </c>
+      <c r="U3">
+        <v>0.99986328499999999</v>
+      </c>
+      <c r="V3">
+        <v>0.99993512900000003</v>
+      </c>
+      <c r="W3">
+        <v>0.99996921999999999</v>
+      </c>
+      <c r="X3">
+        <v>0.99998539600000003</v>
+      </c>
+      <c r="Y3">
+        <v>0.99999307100000001</v>
+      </c>
+      <c r="Z3">
+        <v>0.99999671199999995</v>
+      </c>
+      <c r="AA3">
+        <v>0.99999844000000004</v>
+      </c>
+      <c r="AB3">
+        <v>0.99999925999999995</v>
+      </c>
+      <c r="AC3">
+        <v>0.99999964900000005</v>
+      </c>
+      <c r="AD3">
+        <v>0.99999983299999995</v>
+      </c>
+      <c r="AE3">
+        <v>0.99999992100000001</v>
+      </c>
+      <c r="AF3">
+        <v>0.99999996199999996</v>
+      </c>
+      <c r="AG3">
         <v>0.99999998199999995</v>
       </c>
     </row>
@@ -1023,15 +1167,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1039,97 +1183,100 @@
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1137,94 +1284,198 @@
         <v>49</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>1.2128000000000001</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.5901000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.9759</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.3584000000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2.7286000000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>3.0804999999999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3.41</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3.7149999999999999</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3.9944999999999999</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>4.2485999999999997</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>4.4782000000000002</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>4.6843000000000004</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4.8685999999999998</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>5.0327000000000002</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5.1783999999999999</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>5.3072999999999997</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>5.4210000000000003</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>5.5213000000000001</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>5.6093999999999999</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>5.6867999999999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>5.7545999999999999</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>5.8140999999999998</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>5.8661000000000003</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>5.9115000000000002</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>5.9512</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>5.9859</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>6.0160999999999998</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>6.0425000000000004</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>6.0655000000000001</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>6.1528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.1085</v>
+      </c>
+      <c r="E3">
+        <v>1.4285000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.7228000000000001</v>
+      </c>
+      <c r="G3">
+        <v>1.9837</v>
+      </c>
+      <c r="H3">
+        <v>2.2088999999999999</v>
+      </c>
+      <c r="I3">
+        <v>2.3995000000000002</v>
+      </c>
+      <c r="J3">
+        <v>2.5586000000000002</v>
+      </c>
+      <c r="K3">
+        <v>2.6899000000000002</v>
+      </c>
+      <c r="L3">
+        <v>2.7974000000000001</v>
+      </c>
+      <c r="M3">
+        <v>2.8847999999999998</v>
+      </c>
+      <c r="N3">
+        <v>2.9554999999999998</v>
+      </c>
+      <c r="O3">
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="P3">
+        <v>3.0583999999999998</v>
+      </c>
+      <c r="Q3">
+        <v>3.0951</v>
+      </c>
+      <c r="R3">
+        <v>3.1244999999999998</v>
+      </c>
+      <c r="S3">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="T3">
+        <v>3.1667999999999998</v>
+      </c>
+      <c r="U3">
+        <v>3.1817000000000002</v>
+      </c>
+      <c r="V3">
+        <v>3.1936</v>
+      </c>
+      <c r="W3">
+        <v>3.2031000000000001</v>
+      </c>
+      <c r="X3">
+        <v>3.2107000000000001</v>
+      </c>
+      <c r="Y3">
+        <v>3.2166999999999999</v>
+      </c>
+      <c r="Z3">
+        <v>3.2214999999999998</v>
+      </c>
+      <c r="AA3">
+        <v>3.2252999999999998</v>
+      </c>
+      <c r="AB3">
+        <v>3.2282999999999999</v>
+      </c>
+      <c r="AC3">
+        <v>3.2307000000000001</v>
+      </c>
+      <c r="AD3">
+        <v>3.2326000000000001</v>
+      </c>
+      <c r="AE3">
+        <v>3.2341000000000002</v>
+      </c>
+      <c r="AF3">
+        <v>3.2353000000000001</v>
+      </c>
+      <c r="AG3">
+        <v>3.2381000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1236,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1542,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
incorporating sex and fleet structure into OM
Note that WHAM does not include sex structure. Thus, when we run WHAM, we will need to specify one sex instead of two.

Equilibrium checks have been met. make_input needs to be adjusted to incorporate the new data structures that may have been created
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E843AF4A-9803-064E-9207-0EB62891FDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CCB7E4-BD25-A44F-B04F-EE1A183ED14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>Par</t>
   </si>
@@ -216,10 +216,19 @@
     <t>Number of sexes (1. = Females, 2 = Males)</t>
   </si>
   <si>
-    <t>n_fleets</t>
-  </si>
-  <si>
     <t>Number of fishery fleets</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>n_fish_fleets</t>
+  </si>
+  <si>
+    <t>Number of survey fleets</t>
+  </si>
+  <si>
+    <t>n_srv_fleets</t>
   </si>
 </sst>
 </file>
@@ -585,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -623,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
@@ -645,7 +654,7 @@
         <v>56</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>57</v>
@@ -653,13 +662,24 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +692,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A5" sqref="A5:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,15 +865,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -861,97 +881,100 @@
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -959,93 +982,197 @@
         <v>49</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>2.2375362999999999E-2</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.6018622000000002E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>9.2286517999999998E-2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.176467916</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.31111834199999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.48767028899999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.66735326100000003</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.80873412499999997</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.89910986100000001</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.94945097899999997</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.97536173299999995</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>0.98815665200000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.99434555199999997</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.99730916599999997</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.99872148500000002</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.99939298099999996</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>0.99971189900000001</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.99986328499999999</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>0.99993512900000003</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>0.99996921999999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>0.99998539600000003</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>0.99999307100000001</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>0.99999671199999995</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>0.99999844000000004</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>0.99999925999999995</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>0.99999964900000005</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>0.99999983299999995</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>0.99999992100000001</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>0.99999996199999996</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
+        <v>0.99999998199999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2.2375362999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.6018622000000002E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.2286517999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.176467916</v>
+      </c>
+      <c r="H3">
+        <v>0.31111834199999999</v>
+      </c>
+      <c r="I3">
+        <v>0.48767028899999998</v>
+      </c>
+      <c r="J3">
+        <v>0.66735326100000003</v>
+      </c>
+      <c r="K3">
+        <v>0.80873412499999997</v>
+      </c>
+      <c r="L3">
+        <v>0.89910986100000001</v>
+      </c>
+      <c r="M3">
+        <v>0.94945097899999997</v>
+      </c>
+      <c r="N3">
+        <v>0.97536173299999995</v>
+      </c>
+      <c r="O3">
+        <v>0.98815665200000002</v>
+      </c>
+      <c r="P3">
+        <v>0.99434555199999997</v>
+      </c>
+      <c r="Q3">
+        <v>0.99730916599999997</v>
+      </c>
+      <c r="R3">
+        <v>0.99872148500000002</v>
+      </c>
+      <c r="S3">
+        <v>0.99939298099999996</v>
+      </c>
+      <c r="T3">
+        <v>0.99971189900000001</v>
+      </c>
+      <c r="U3">
+        <v>0.99986328499999999</v>
+      </c>
+      <c r="V3">
+        <v>0.99993512900000003</v>
+      </c>
+      <c r="W3">
+        <v>0.99996921999999999</v>
+      </c>
+      <c r="X3">
+        <v>0.99998539600000003</v>
+      </c>
+      <c r="Y3">
+        <v>0.99999307100000001</v>
+      </c>
+      <c r="Z3">
+        <v>0.99999671199999995</v>
+      </c>
+      <c r="AA3">
+        <v>0.99999844000000004</v>
+      </c>
+      <c r="AB3">
+        <v>0.99999925999999995</v>
+      </c>
+      <c r="AC3">
+        <v>0.99999964900000005</v>
+      </c>
+      <c r="AD3">
+        <v>0.99999983299999995</v>
+      </c>
+      <c r="AE3">
+        <v>0.99999992100000001</v>
+      </c>
+      <c r="AF3">
+        <v>0.99999996199999996</v>
+      </c>
+      <c r="AG3">
         <v>0.99999998199999995</v>
       </c>
     </row>
@@ -1057,15 +1184,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1073,97 +1200,100 @@
         <v>48</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1171,94 +1301,198 @@
         <v>49</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>1.2128000000000001</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.5901000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.9759</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.3584000000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2.7286000000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>3.0804999999999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3.41</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3.7149999999999999</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3.9944999999999999</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>4.2485999999999997</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>4.4782000000000002</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>4.6843000000000004</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4.8685999999999998</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>5.0327000000000002</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5.1783999999999999</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>5.3072999999999997</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>5.4210000000000003</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>5.5213000000000001</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>5.6093999999999999</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>5.6867999999999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>5.7545999999999999</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>5.8140999999999998</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>5.8661000000000003</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>5.9115000000000002</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>5.9512</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>5.9859</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>6.0160999999999998</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>6.0425000000000004</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>6.0655000000000001</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>6.1528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.1085</v>
+      </c>
+      <c r="E3">
+        <v>1.4285000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.7228000000000001</v>
+      </c>
+      <c r="G3">
+        <v>1.9837</v>
+      </c>
+      <c r="H3">
+        <v>2.2088999999999999</v>
+      </c>
+      <c r="I3">
+        <v>2.3995000000000002</v>
+      </c>
+      <c r="J3">
+        <v>2.5586000000000002</v>
+      </c>
+      <c r="K3">
+        <v>2.6899000000000002</v>
+      </c>
+      <c r="L3">
+        <v>2.7974000000000001</v>
+      </c>
+      <c r="M3">
+        <v>2.8847999999999998</v>
+      </c>
+      <c r="N3">
+        <v>2.9554999999999998</v>
+      </c>
+      <c r="O3">
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="P3">
+        <v>3.0583999999999998</v>
+      </c>
+      <c r="Q3">
+        <v>3.0951</v>
+      </c>
+      <c r="R3">
+        <v>3.1244999999999998</v>
+      </c>
+      <c r="S3">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="T3">
+        <v>3.1667999999999998</v>
+      </c>
+      <c r="U3">
+        <v>3.1817000000000002</v>
+      </c>
+      <c r="V3">
+        <v>3.1936</v>
+      </c>
+      <c r="W3">
+        <v>3.2031000000000001</v>
+      </c>
+      <c r="X3">
+        <v>3.2107000000000001</v>
+      </c>
+      <c r="Y3">
+        <v>3.2166999999999999</v>
+      </c>
+      <c r="Z3">
+        <v>3.2214999999999998</v>
+      </c>
+      <c r="AA3">
+        <v>3.2252999999999998</v>
+      </c>
+      <c r="AB3">
+        <v>3.2282999999999999</v>
+      </c>
+      <c r="AC3">
+        <v>3.2307000000000001</v>
+      </c>
+      <c r="AD3">
+        <v>3.2326000000000001</v>
+      </c>
+      <c r="AE3">
+        <v>3.2341000000000002</v>
+      </c>
+      <c r="AF3">
+        <v>3.2353000000000001</v>
+      </c>
+      <c r="AG3">
+        <v>3.2381000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1270,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1325,7 +1559,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
updating sim code + convergence checks
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CCB7E4-BD25-A44F-B04F-EE1A183ED14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79753435-E03E-514C-82BA-6B7765DC7101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>Par</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Number of simulations</t>
-  </si>
-  <si>
     <t>ages</t>
   </si>
   <si>
@@ -84,158 +81,161 @@
     <t>r0</t>
   </si>
   <si>
+    <t>sigma_rec</t>
+  </si>
+  <si>
+    <t>Recruitment variability</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time_Inv</t>
+  </si>
+  <si>
+    <t>Number of years (clipping off the last year)</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Natural Mortality</t>
+  </si>
+  <si>
+    <t>Mean recruitment</t>
+  </si>
+  <si>
+    <t>mu_rec</t>
+  </si>
+  <si>
+    <t>n_sex</t>
+  </si>
+  <si>
+    <t>Number of sexes (1. = Females, 2 = Males)</t>
+  </si>
+  <si>
+    <t>Number of fishery fleets</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>n_fish_fleets</t>
+  </si>
+  <si>
+    <t>Number of survey fleets</t>
+  </si>
+  <si>
+    <t>n_srv_fleets</t>
+  </si>
+  <si>
+    <t>Steepness (taken from .pin of SAFE - not sure if this is really correct)</t>
+  </si>
+  <si>
+    <t>Recruitment at unfished equilibrium (using halibut values)</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a13</t>
+  </si>
+  <si>
+    <t>a14</t>
+  </si>
+  <si>
+    <t>a15</t>
+  </si>
+  <si>
+    <t>a16</t>
+  </si>
+  <si>
+    <t>a17</t>
+  </si>
+  <si>
+    <t>a18</t>
+  </si>
+  <si>
+    <t>a19</t>
+  </si>
+  <si>
+    <t>a20</t>
+  </si>
+  <si>
+    <t>a21</t>
+  </si>
+  <si>
+    <t>a22</t>
+  </si>
+  <si>
+    <t>a23</t>
+  </si>
+  <si>
+    <t>a24</t>
+  </si>
+  <si>
+    <t>a25</t>
+  </si>
+  <si>
+    <t>a26</t>
+  </si>
+  <si>
+    <t>a27</t>
+  </si>
+  <si>
+    <t>a28</t>
+  </si>
+  <si>
+    <t>a29</t>
+  </si>
+  <si>
+    <t>a30</t>
+  </si>
+  <si>
+    <t>a31</t>
+  </si>
+  <si>
+    <t>Number of simulations (Some general notes: Weight at age are based off only females - these are genearlized single sex inputs)</t>
+  </si>
+  <si>
     <t>ssb0</t>
   </si>
   <si>
-    <t>sigma_rec</t>
-  </si>
-  <si>
-    <t>Recruitment variability</t>
-  </si>
-  <si>
-    <t>SSB at unfished equilibrium</t>
-  </si>
-  <si>
-    <t>Steepness</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a5</t>
-  </si>
-  <si>
-    <t>a6</t>
-  </si>
-  <si>
-    <t>a7</t>
-  </si>
-  <si>
-    <t>a8</t>
-  </si>
-  <si>
-    <t>a9</t>
-  </si>
-  <si>
-    <t>a10</t>
-  </si>
-  <si>
-    <t>a11</t>
-  </si>
-  <si>
-    <t>a12</t>
-  </si>
-  <si>
-    <t>a13</t>
-  </si>
-  <si>
-    <t>a14</t>
-  </si>
-  <si>
-    <t>a15</t>
-  </si>
-  <si>
-    <t>a16</t>
-  </si>
-  <si>
-    <t>a17</t>
-  </si>
-  <si>
-    <t>a18</t>
-  </si>
-  <si>
-    <t>a19</t>
-  </si>
-  <si>
-    <t>a20</t>
-  </si>
-  <si>
-    <t>a21</t>
-  </si>
-  <si>
-    <t>a22</t>
-  </si>
-  <si>
-    <t>a23</t>
-  </si>
-  <si>
-    <t>a24</t>
-  </si>
-  <si>
-    <t>a25</t>
-  </si>
-  <si>
-    <t>a26</t>
-  </si>
-  <si>
-    <t>a27</t>
-  </si>
-  <si>
-    <t>a28</t>
-  </si>
-  <si>
-    <t>a29</t>
-  </si>
-  <si>
-    <t>a30</t>
-  </si>
-  <si>
-    <t>a31</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Time_Inv</t>
-  </si>
-  <si>
-    <t>Recruitment at unfished equilibrium (taken from starting values of .dat file) - exponentiated</t>
-  </si>
-  <si>
-    <t>Number of years (clipping off the last year)</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Natural Mortality</t>
-  </si>
-  <si>
-    <t>Mean recruitment</t>
-  </si>
-  <si>
-    <t>mu_rec</t>
-  </si>
-  <si>
-    <t>n_sex</t>
-  </si>
-  <si>
-    <t>Number of sexes (1. = Females, 2 = Males)</t>
-  </si>
-  <si>
-    <t>Number of fishery fleets</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>n_fish_fleets</t>
-  </si>
-  <si>
-    <t>Number of survey fleets</t>
-  </si>
-  <si>
-    <t>n_srv_fleets</t>
+    <t>Virgin SSB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -245,13 +245,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,9 +270,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,10 +613,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -632,54 +624,54 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -692,14 +684,14 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A31"/>
+      <selection activeCell="A13" sqref="A13:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -710,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -865,113 +857,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="O1" sqref="O1:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="V1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -979,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1072,107 +1064,6 @@
         <v>0.99999996199999996</v>
       </c>
       <c r="AG2">
-        <v>0.99999998199999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2.2375362999999999E-2</v>
-      </c>
-      <c r="E3">
-        <v>4.6018622000000002E-2</v>
-      </c>
-      <c r="F3">
-        <v>9.2286517999999998E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.176467916</v>
-      </c>
-      <c r="H3">
-        <v>0.31111834199999999</v>
-      </c>
-      <c r="I3">
-        <v>0.48767028899999998</v>
-      </c>
-      <c r="J3">
-        <v>0.66735326100000003</v>
-      </c>
-      <c r="K3">
-        <v>0.80873412499999997</v>
-      </c>
-      <c r="L3">
-        <v>0.89910986100000001</v>
-      </c>
-      <c r="M3">
-        <v>0.94945097899999997</v>
-      </c>
-      <c r="N3">
-        <v>0.97536173299999995</v>
-      </c>
-      <c r="O3">
-        <v>0.98815665200000002</v>
-      </c>
-      <c r="P3">
-        <v>0.99434555199999997</v>
-      </c>
-      <c r="Q3">
-        <v>0.99730916599999997</v>
-      </c>
-      <c r="R3">
-        <v>0.99872148500000002</v>
-      </c>
-      <c r="S3">
-        <v>0.99939298099999996</v>
-      </c>
-      <c r="T3">
-        <v>0.99971189900000001</v>
-      </c>
-      <c r="U3">
-        <v>0.99986328499999999</v>
-      </c>
-      <c r="V3">
-        <v>0.99993512900000003</v>
-      </c>
-      <c r="W3">
-        <v>0.99996921999999999</v>
-      </c>
-      <c r="X3">
-        <v>0.99998539600000003</v>
-      </c>
-      <c r="Y3">
-        <v>0.99999307100000001</v>
-      </c>
-      <c r="Z3">
-        <v>0.99999671199999995</v>
-      </c>
-      <c r="AA3">
-        <v>0.99999844000000004</v>
-      </c>
-      <c r="AB3">
-        <v>0.99999925999999995</v>
-      </c>
-      <c r="AC3">
-        <v>0.99999964900000005</v>
-      </c>
-      <c r="AD3">
-        <v>0.99999983299999995</v>
-      </c>
-      <c r="AE3">
-        <v>0.99999992100000001</v>
-      </c>
-      <c r="AF3">
-        <v>0.99999996199999996</v>
-      </c>
-      <c r="AG3">
         <v>0.99999998199999995</v>
       </c>
     </row>
@@ -1184,318 +1075,218 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="B1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="W1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="X1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.2128000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.5901000000000001</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1.9759</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2.3584000000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2.7286000000000001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3.0804999999999998</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3.41</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3.7149999999999999</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>3.9944999999999999</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>4.2485999999999997</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>4.4782000000000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>4.6843000000000004</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>4.8685999999999998</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5.0327000000000002</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>5.1783999999999999</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>5.3072999999999997</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>5.4210000000000003</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>5.5213000000000001</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>5.6093999999999999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>5.6867999999999999</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>5.7545999999999999</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>5.8140999999999998</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>5.8661000000000003</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>5.9115000000000002</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>5.9512</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>5.9859</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>6.0160999999999998</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>6.0425000000000004</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>6.0655000000000001</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>6.1528</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1.1085</v>
-      </c>
-      <c r="E3">
-        <v>1.4285000000000001</v>
-      </c>
-      <c r="F3">
-        <v>1.7228000000000001</v>
-      </c>
-      <c r="G3">
-        <v>1.9837</v>
-      </c>
-      <c r="H3">
-        <v>2.2088999999999999</v>
-      </c>
-      <c r="I3">
-        <v>2.3995000000000002</v>
-      </c>
-      <c r="J3">
-        <v>2.5586000000000002</v>
-      </c>
-      <c r="K3">
-        <v>2.6899000000000002</v>
-      </c>
-      <c r="L3">
-        <v>2.7974000000000001</v>
-      </c>
-      <c r="M3">
-        <v>2.8847999999999998</v>
-      </c>
-      <c r="N3">
-        <v>2.9554999999999998</v>
-      </c>
-      <c r="O3">
-        <v>3.0125000000000002</v>
-      </c>
-      <c r="P3">
-        <v>3.0583999999999998</v>
-      </c>
-      <c r="Q3">
-        <v>3.0951</v>
-      </c>
-      <c r="R3">
-        <v>3.1244999999999998</v>
-      </c>
-      <c r="S3">
-        <v>3.1480000000000001</v>
-      </c>
-      <c r="T3">
-        <v>3.1667999999999998</v>
-      </c>
-      <c r="U3">
-        <v>3.1817000000000002</v>
-      </c>
-      <c r="V3">
-        <v>3.1936</v>
-      </c>
-      <c r="W3">
-        <v>3.2031000000000001</v>
-      </c>
-      <c r="X3">
-        <v>3.2107000000000001</v>
-      </c>
-      <c r="Y3">
-        <v>3.2166999999999999</v>
-      </c>
-      <c r="Z3">
-        <v>3.2214999999999998</v>
-      </c>
-      <c r="AA3">
-        <v>3.2252999999999998</v>
-      </c>
-      <c r="AB3">
-        <v>3.2282999999999999</v>
-      </c>
-      <c r="AC3">
-        <v>3.2307000000000001</v>
-      </c>
-      <c r="AD3">
-        <v>3.2326000000000001</v>
-      </c>
-      <c r="AE3">
-        <v>3.2341000000000002</v>
-      </c>
-      <c r="AF3">
-        <v>3.2353000000000001</v>
-      </c>
-      <c r="AG3">
-        <v>3.2381000000000002</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1504,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1523,68 +1314,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>0.59950000000000003</v>
+        <v>0.59955000000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>20.085540000000002</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4">
-        <v>246.28489999999999</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>1.2</v>
+        <v>0.10061036447831166</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.1</v>
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>1.6</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B7">
-        <v>16.5</v>
+        <v>100.2134123</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tmb model - first commit
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79753435-E03E-514C-82BA-6B7765DC7101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E463BB-543A-1041-98E7-3AB11DFABB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>Par</t>
   </si>
@@ -60,9 +60,6 @@
     <t>ages</t>
   </si>
   <si>
-    <t>Age 2 is the recruitment age, age 31 is the plus group</t>
-  </si>
-  <si>
     <t>N_1</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>a30</t>
   </si>
   <si>
-    <t>a31</t>
-  </si>
-  <si>
     <t>Number of simulations (Some general notes: Weight at age are based off only females - these are genearlized single sex inputs)</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t>Virgin SSB</t>
+  </si>
+  <si>
+    <t>a1</t>
   </si>
 </sst>
 </file>
@@ -290,7 +287,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -578,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,10 +610,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -627,51 +624,51 @@
         <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +681,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,155 +696,152 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -860,110 +854,110 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:AG2"/>
+      <selection activeCell="D1" sqref="D1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>49</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>55</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>56</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>57</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -971,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1075,213 +1069,213 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="B1:AH2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AI2"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" t="s">
-        <v>46</v>
-      </c>
-      <c r="V1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.2128000000000001</v>
       </c>
       <c r="E2">
-        <v>1.2128000000000001</v>
+        <v>1.5901000000000001</v>
       </c>
       <c r="F2">
-        <v>1.5901000000000001</v>
+        <v>1.9759</v>
       </c>
       <c r="G2">
-        <v>1.9759</v>
+        <v>2.3584000000000001</v>
       </c>
       <c r="H2">
-        <v>2.3584000000000001</v>
+        <v>2.7286000000000001</v>
       </c>
       <c r="I2">
-        <v>2.7286000000000001</v>
+        <v>3.0804999999999998</v>
       </c>
       <c r="J2">
-        <v>3.0804999999999998</v>
+        <v>3.41</v>
       </c>
       <c r="K2">
-        <v>3.41</v>
+        <v>3.7149999999999999</v>
       </c>
       <c r="L2">
-        <v>3.7149999999999999</v>
+        <v>3.9944999999999999</v>
       </c>
       <c r="M2">
-        <v>3.9944999999999999</v>
+        <v>4.2485999999999997</v>
       </c>
       <c r="N2">
-        <v>4.2485999999999997</v>
+        <v>4.4782000000000002</v>
       </c>
       <c r="O2">
-        <v>4.4782000000000002</v>
+        <v>4.6843000000000004</v>
       </c>
       <c r="P2">
-        <v>4.6843000000000004</v>
+        <v>4.8685999999999998</v>
       </c>
       <c r="Q2">
-        <v>4.8685999999999998</v>
+        <v>5.0327000000000002</v>
       </c>
       <c r="R2">
-        <v>5.0327000000000002</v>
+        <v>5.1783999999999999</v>
       </c>
       <c r="S2">
-        <v>5.1783999999999999</v>
+        <v>5.3072999999999997</v>
       </c>
       <c r="T2">
-        <v>5.3072999999999997</v>
+        <v>5.4210000000000003</v>
       </c>
       <c r="U2">
-        <v>5.4210000000000003</v>
+        <v>5.5213000000000001</v>
       </c>
       <c r="V2">
-        <v>5.5213000000000001</v>
+        <v>5.6093999999999999</v>
       </c>
       <c r="W2">
-        <v>5.6093999999999999</v>
+        <v>5.6867999999999999</v>
       </c>
       <c r="X2">
-        <v>5.6867999999999999</v>
+        <v>5.7545999999999999</v>
       </c>
       <c r="Y2">
-        <v>5.7545999999999999</v>
+        <v>5.8140999999999998</v>
       </c>
       <c r="Z2">
-        <v>5.8140999999999998</v>
+        <v>5.8661000000000003</v>
       </c>
       <c r="AA2">
-        <v>5.8661000000000003</v>
+        <v>5.9115000000000002</v>
       </c>
       <c r="AB2">
-        <v>5.9115000000000002</v>
+        <v>5.9512</v>
       </c>
       <c r="AC2">
-        <v>5.9512</v>
+        <v>5.9859</v>
       </c>
       <c r="AD2">
-        <v>5.9859</v>
+        <v>6.0160999999999998</v>
       </c>
       <c r="AE2">
-        <v>6.0160999999999998</v>
+        <v>6.0425000000000004</v>
       </c>
       <c r="AF2">
-        <v>6.0425000000000004</v>
+        <v>6.0655000000000001</v>
       </c>
       <c r="AG2">
-        <v>6.0655000000000001</v>
-      </c>
-      <c r="AH2">
         <v>6.1528</v>
       </c>
     </row>
@@ -1295,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1314,68 +1308,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.59955000000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>20.085540000000002</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1.2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0.125</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
-      </c>
-      <c r="B5">
-        <v>0.10061036447831166</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>1.6</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>100.2134123</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
incorporate survey comp info + penalize like for recdevs
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E463BB-543A-1041-98E7-3AB11DFABB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E314B-B049-7A41-913F-E309157E52FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -1290,7 +1290,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.05</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
resolved recruitment penalty and init at age woes....
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E314B-B049-7A41-913F-E309157E52FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E725045-75AB-204A-8693-3EB9661E4DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>0.7</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
model validation - still working but saving new version of .cpp
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E725045-75AB-204A-8693-3EB9661E4DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C026431-D6D9-EC4E-BA5F-9432A6DC5A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="AH1" sqref="AH1:AH1048576"/>
     </sheetView>
   </sheetViews>
@@ -1289,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1344,7 +1344,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
breakthrough!!! removed biased estimates, and have relatively unbiased estimates now!
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C026431-D6D9-EC4E-BA5F-9432A6DC5A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73C204E-4366-1F4A-AA8A-5AFEB9D14350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -1290,7 +1290,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1344,7 +1344,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1355,7 +1355,7 @@
         <v>28</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
fixing q in loop
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73C204E-4366-1F4A-AA8A-5AFEB9D14350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C777266C-9FC8-B14A-9733-C9BAC2CF497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
adding new summary stats (mean ages)
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C777266C-9FC8-B14A-9733-C9BAC2CF497A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764B65D1-D975-E14D-A74D-19DBD3009D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1289,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding double logistic fxn in EM
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A097FB-C960-3448-825E-5A5503C5A611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914F0C6-DBA9-D248-B5E9-DDD0058A8B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -610,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
hotfix for double logistic, validated 2 fleet structure, and adding data indicators for nLL fitting
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914F0C6-DBA9-D248-B5E9-DDD0058A8B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3F8E21-7153-9243-9951-79BCE320C578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -653,7 +653,7 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
fix for calculating mean ages
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3F8E21-7153-9243-9951-79BCE320C578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379EBCD7-AEA8-8C4D-81DA-107DC7F65DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
cleaning and builiding utlity fxns to run EM
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379EBCD7-AEA8-8C4D-81DA-107DC7F65DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665465A8-F72F-2146-B4F7-C52F35163933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -574,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1332,7 +1332,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
testing ar1_y and 2dar1
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665465A8-F72F-2146-B4F7-C52F35163933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7D7F91-9A8A-A84C-88C9-9C2E9FD2A416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -680,7 +680,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A14" sqref="A14:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:AG1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AH1048576"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding age blocks for 2dar1
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7D7F91-9A8A-A84C-88C9-9C2E9FD2A416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1697842-D348-E64B-89A5-751BEBAB4B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
constrain rhos to -1 and 1, and rerun models
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1697842-D348-E64B-89A5-751BEBAB4B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB290A-F3AC-B742-A209-2E24C09555B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
adding exponential logistic and code cleaning
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FB290A-F3AC-B742-A209-2E24C09555B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E9F151-4DCA-A345-9FAF-9A935DC9B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1288,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1332,7 +1332,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1343,7 +1343,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
verifying 2 fleet 2 sex OM EM
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E9F151-4DCA-A345-9FAF-9A935DC9B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6225283-5C51-5649-AACB-857E556D222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>Par</t>
   </si>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -642,7 +642,7 @@
         <v>29</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -850,10 +850,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AG2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1057,6 +1057,107 @@
         <v>0.99999996199999996</v>
       </c>
       <c r="AG2">
+        <v>0.99999998199999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2.2375362999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.6018622000000002E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.2286517999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.176467916</v>
+      </c>
+      <c r="H3">
+        <v>0.31111834199999999</v>
+      </c>
+      <c r="I3">
+        <v>0.48767028899999998</v>
+      </c>
+      <c r="J3">
+        <v>0.66735326100000003</v>
+      </c>
+      <c r="K3">
+        <v>0.80873412499999997</v>
+      </c>
+      <c r="L3">
+        <v>0.89910986100000001</v>
+      </c>
+      <c r="M3">
+        <v>0.94945097899999997</v>
+      </c>
+      <c r="N3">
+        <v>0.97536173299999995</v>
+      </c>
+      <c r="O3">
+        <v>0.98815665200000002</v>
+      </c>
+      <c r="P3">
+        <v>0.99434555199999997</v>
+      </c>
+      <c r="Q3">
+        <v>0.99730916599999997</v>
+      </c>
+      <c r="R3">
+        <v>0.99872148500000002</v>
+      </c>
+      <c r="S3">
+        <v>0.99939298099999996</v>
+      </c>
+      <c r="T3">
+        <v>0.99971189900000001</v>
+      </c>
+      <c r="U3">
+        <v>0.99986328499999999</v>
+      </c>
+      <c r="V3">
+        <v>0.99993512900000003</v>
+      </c>
+      <c r="W3">
+        <v>0.99996921999999999</v>
+      </c>
+      <c r="X3">
+        <v>0.99998539600000003</v>
+      </c>
+      <c r="Y3">
+        <v>0.99999307100000001</v>
+      </c>
+      <c r="Z3">
+        <v>0.99999671199999995</v>
+      </c>
+      <c r="AA3">
+        <v>0.99999844000000004</v>
+      </c>
+      <c r="AB3">
+        <v>0.99999925999999995</v>
+      </c>
+      <c r="AC3">
+        <v>0.99999964900000005</v>
+      </c>
+      <c r="AD3">
+        <v>0.99999983299999995</v>
+      </c>
+      <c r="AE3">
+        <v>0.99999992100000001</v>
+      </c>
+      <c r="AF3">
+        <v>0.99999996199999996</v>
+      </c>
+      <c r="AG3">
         <v>0.99999998199999995</v>
       </c>
     </row>
@@ -1068,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AG2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,6 +1376,107 @@
         <v>6.0655000000000001</v>
       </c>
       <c r="AG2">
+        <v>6.1528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1.2128000000000001</v>
+      </c>
+      <c r="E3">
+        <v>1.5901000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.9759</v>
+      </c>
+      <c r="G3">
+        <v>2.3584000000000001</v>
+      </c>
+      <c r="H3">
+        <v>2.7286000000000001</v>
+      </c>
+      <c r="I3">
+        <v>3.0804999999999998</v>
+      </c>
+      <c r="J3">
+        <v>3.41</v>
+      </c>
+      <c r="K3">
+        <v>3.7149999999999999</v>
+      </c>
+      <c r="L3">
+        <v>3.9944999999999999</v>
+      </c>
+      <c r="M3">
+        <v>4.2485999999999997</v>
+      </c>
+      <c r="N3">
+        <v>4.4782000000000002</v>
+      </c>
+      <c r="O3">
+        <v>4.6843000000000004</v>
+      </c>
+      <c r="P3">
+        <v>4.8685999999999998</v>
+      </c>
+      <c r="Q3">
+        <v>5.0327000000000002</v>
+      </c>
+      <c r="R3">
+        <v>5.1783999999999999</v>
+      </c>
+      <c r="S3">
+        <v>5.3072999999999997</v>
+      </c>
+      <c r="T3">
+        <v>5.4210000000000003</v>
+      </c>
+      <c r="U3">
+        <v>5.5213000000000001</v>
+      </c>
+      <c r="V3">
+        <v>5.6093999999999999</v>
+      </c>
+      <c r="W3">
+        <v>5.6867999999999999</v>
+      </c>
+      <c r="X3">
+        <v>5.7545999999999999</v>
+      </c>
+      <c r="Y3">
+        <v>5.8140999999999998</v>
+      </c>
+      <c r="Z3">
+        <v>5.8661000000000003</v>
+      </c>
+      <c r="AA3">
+        <v>5.9115000000000002</v>
+      </c>
+      <c r="AB3">
+        <v>5.9512</v>
+      </c>
+      <c r="AC3">
+        <v>5.9859</v>
+      </c>
+      <c r="AD3">
+        <v>6.0160999999999998</v>
+      </c>
+      <c r="AE3">
+        <v>6.0425000000000004</v>
+      </c>
+      <c r="AF3">
+        <v>6.0655000000000001</v>
+      </c>
+      <c r="AG3">
         <v>6.1528</v>
       </c>
     </row>
@@ -1288,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish verifying sex-specific model
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6225283-5C51-5649-AACB-857E556D222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0256C347-546F-024F-BDAE-E43A647DFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing waa indexing for 2 sex
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0256C347-546F-024F-BDAE-E43A647DFF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F15748-61AA-034B-B187-97505A306B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +241,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,8 +273,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -852,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,95 +1398,185 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1.2128000000000001</v>
+        <v>1.1085</v>
       </c>
       <c r="E3">
-        <v>1.5901000000000001</v>
+        <v>1.4285000000000001</v>
       </c>
       <c r="F3">
-        <v>1.9759</v>
+        <v>1.7228000000000001</v>
       </c>
       <c r="G3">
-        <v>2.3584000000000001</v>
+        <v>1.9837</v>
       </c>
       <c r="H3">
-        <v>2.7286000000000001</v>
+        <v>2.2088999999999999</v>
       </c>
       <c r="I3">
-        <v>3.0804999999999998</v>
+        <v>2.3995000000000002</v>
       </c>
       <c r="J3">
-        <v>3.41</v>
+        <v>2.5586000000000002</v>
       </c>
       <c r="K3">
-        <v>3.7149999999999999</v>
+        <v>2.6899000000000002</v>
       </c>
       <c r="L3">
-        <v>3.9944999999999999</v>
+        <v>2.7974000000000001</v>
       </c>
       <c r="M3">
-        <v>4.2485999999999997</v>
+        <v>2.8847999999999998</v>
       </c>
       <c r="N3">
-        <v>4.4782000000000002</v>
+        <v>2.9554999999999998</v>
       </c>
       <c r="O3">
-        <v>4.6843000000000004</v>
+        <v>3.0125000000000002</v>
       </c>
       <c r="P3">
-        <v>4.8685999999999998</v>
+        <v>3.0583999999999998</v>
       </c>
       <c r="Q3">
-        <v>5.0327000000000002</v>
+        <v>3.0951</v>
       </c>
       <c r="R3">
-        <v>5.1783999999999999</v>
+        <v>3.1244999999999998</v>
       </c>
       <c r="S3">
-        <v>5.3072999999999997</v>
+        <v>3.1480000000000001</v>
       </c>
       <c r="T3">
-        <v>5.4210000000000003</v>
+        <v>3.1667999999999998</v>
       </c>
       <c r="U3">
-        <v>5.5213000000000001</v>
+        <v>3.1817000000000002</v>
       </c>
       <c r="V3">
-        <v>5.6093999999999999</v>
+        <v>3.1936</v>
       </c>
       <c r="W3">
-        <v>5.6867999999999999</v>
+        <v>3.2031000000000001</v>
       </c>
       <c r="X3">
-        <v>5.7545999999999999</v>
+        <v>3.2107000000000001</v>
       </c>
       <c r="Y3">
-        <v>5.8140999999999998</v>
+        <v>3.2166999999999999</v>
       </c>
       <c r="Z3">
-        <v>5.8661000000000003</v>
+        <v>3.2214999999999998</v>
       </c>
       <c r="AA3">
-        <v>5.9115000000000002</v>
+        <v>3.2252999999999998</v>
       </c>
       <c r="AB3">
-        <v>5.9512</v>
+        <v>3.2282999999999999</v>
       </c>
       <c r="AC3">
-        <v>5.9859</v>
+        <v>3.2307000000000001</v>
       </c>
       <c r="AD3">
-        <v>6.0160999999999998</v>
+        <v>3.2326000000000001</v>
       </c>
       <c r="AE3">
-        <v>6.0425000000000004</v>
+        <v>3.2341000000000002</v>
       </c>
       <c r="AF3">
-        <v>6.0655000000000001</v>
+        <v>3.2353000000000001</v>
       </c>
       <c r="AG3">
-        <v>6.1528</v>
-      </c>
+        <v>3.2381000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixed OM to get catch correct
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F15748-61AA-034B-B187-97505A306B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF512BB5-3656-234A-9A39-DE9A63506DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -860,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding time-varying options in EM inputs
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF512BB5-3656-234A-9A39-DE9A63506DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB4BE5-1F11-C249-8CB8-D735D4AF6375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
adding Bevy Holt into OM and EM!
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CB4BE5-1F11-C249-8CB8-D735D4AF6375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E15A0A-8CE3-4A40-B6B1-3689B1AB18EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>Par</t>
   </si>
@@ -149,9 +149,6 @@
     <t>n_srv_fleets</t>
   </si>
   <si>
-    <t>Steepness (taken from .pin of SAFE - not sure if this is really correct)</t>
-  </si>
-  <si>
     <t>Recruitment at unfished equilibrium (using halibut values)</t>
   </si>
   <si>
@@ -218,13 +215,10 @@
     <t>Number of simulations (Some general notes: Weight at age are based off only females - these are genearlized single sex inputs)</t>
   </si>
   <si>
-    <t>ssb0</t>
-  </si>
-  <si>
-    <t>Virgin SSB</t>
-  </si>
-  <si>
     <t>a1</t>
+  </si>
+  <si>
+    <t>Arbritary steepness value</t>
   </si>
 </sst>
 </file>
@@ -592,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -617,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -877,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -907,64 +901,64 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1196,7 +1190,7 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -1226,64 +1220,64 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>52</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>56</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -1586,9 +1580,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1610,10 +1604,10 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.59955000000000003</v>
+        <v>0.7</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1621,10 +1615,10 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>20.085540000000002</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1658,17 +1652,6 @@
       </c>
       <c r="C6" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7">
-        <v>100.2134123</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding walleye pollock life history
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/State_Space_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E15A0A-8CE3-4A40-B6B1-3689B1AB18EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A386AD50-925D-514B-A3AF-30E567DAAC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>n_srv_fleets</t>
   </si>
   <si>
-    <t>Recruitment at unfished equilibrium (using halibut values)</t>
-  </si>
-  <si>
     <t>a11</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>Arbritary steepness value</t>
+  </si>
+  <si>
+    <t>Recruitment at unfished equilibrium</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -871,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -901,64 +901,64 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>42</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>45</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>55</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1190,7 +1190,7 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -1220,64 +1220,64 @@
         <v>20</v>
       </c>
       <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>42</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>44</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>45</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>55</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -1583,7 +1583,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,10 +1604,10 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.7</v>
+        <v>0.59955000000000003</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1615,10 +1615,10 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
ln_sigmaRec in likelihood instead of exponent of sigr.. seems to fix issues w/ rec
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C9BCFD-373F-4547-A5A5-A49FF5449D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B77164-3BDC-B849-A23D-D2603508ABF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
@@ -1637,7 +1637,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
LETS GO! figured recruitment out!
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7520CF5F-123C-B94D-B462-08100C0113F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B3FFC6-8D24-2B4F-A13F-90E77D14C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -633,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1583,7 +1583,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1615,7 +1615,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>15.64263</v>
+        <v>17.287780000000001</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
@@ -1637,7 +1637,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -1648,7 +1648,7 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>2.75</v>
+        <v>2.85</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
fixed rowsums for OM ZAA_s, and SSB calcualtions
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36B765E-08A5-AC4A-A110-0672AA9F321E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892A2271-E120-5749-AD9A-ABAD6D27DC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -587,7 +587,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -622,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -1637,7 +1637,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.14499999999999999</v>
+        <v>0.108</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
i dont even know anymore
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC37825-BEB1-DC4B-94EC-7C0A693FFC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00B3DF7-493F-3B46-85CA-8D50B04334C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="239" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -1583,7 +1583,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1626,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.05</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
selex des as independent parameters
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B126A425-A985-E444-AE71-9309A2867129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6322F2F6-15BF-4348-ABFC-3E6D875A6B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="239" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="239" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
wooo! unbiased checks are finally done
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6322F2F6-15BF-4348-ABFC-3E6D875A6B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38E7B83-A915-044A-9FE1-2946EDD5E9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="239" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
saving work and adding OM data files
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2748CD7-5F79-9144-918D-AFD04029C585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9F5DCB-457E-EE43-A917-03D8F4F6598E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
@@ -622,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
updating some quick stuff
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9F5DCB-457E-EE43-A917-03D8F4F6598E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A38A486-C298-D949-9AA1-0D2964B15FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Par</t>
   </si>
@@ -47,9 +47,6 @@
     <t>n_sims</t>
   </si>
   <si>
-    <t>n_years</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>Time_Inv</t>
-  </si>
-  <si>
-    <t>Number of years (clipping off the last year)</t>
   </si>
   <si>
     <t>M</t>
@@ -584,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,10 +594,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -614,40 +608,40 @@
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -655,21 +649,10 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -689,10 +672,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -862,103 +845,103 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
       <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>42</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>50</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -966,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1067,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1181,103 +1164,103 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
       <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>40</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>41</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>42</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>47</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>48</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>50</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -1285,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1386,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1593,65 +1576,65 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>17.287780000000001</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0.8</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0.108</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>2.85</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>